<commit_message>
Update SmokeProofScenario template file 1. 去除单元格内的数据验证 2. 去除sheet的编号
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/DesignData/SmokeProofScenario.xlsx
+++ b/AutoLoader/Contents/Support/DesignData/SmokeProofScenario.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\Git\AutoLoader\Contents\Support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BaiduNetdiskDownload\产品开发\01_暖通\02_防烟计算（消防加压送风）\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="782" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="782" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="消防电梯前室" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <definedName name="valveAf">消防电梯前室!#REF!</definedName>
     <definedName name="Width_Valve">消防电梯前室!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="95">
   <si>
     <t>系统名称</t>
   </si>
@@ -695,78 +695,6 @@
   </si>
   <si>
     <t>Type_Door_Q2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前室疏散门3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Width_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Height_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Count_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Count_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>楼梯间疏散门3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Count_Door_L1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Width_Door_L3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Height_Door_L3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Count_Door_L3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Width_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crack_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Height_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crack_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type_Door_Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前室疏散门2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Height_Door_Q3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1021,6 +949,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1034,16 +968,10 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1326,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -1341,21 +1269,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -1365,64 +1293,64 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="4"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="4"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="9"/>
       <c r="F5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="9"/>
       <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="9"/>
       <c r="F8" s="1" t="s">
         <v>40</v>
@@ -1484,10 +1412,10 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="27"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="2"/>
       <c r="D14" s="10"/>
       <c r="F14" s="1" t="s">
@@ -1501,10 +1429,10 @@
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="11"/>
       <c r="F15" s="1" t="s">
         <v>25</v>
@@ -1512,10 +1440,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3"/>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="11"/>
       <c r="F16" t="s">
         <v>26</v>
@@ -1523,10 +1451,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2"/>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="11"/>
       <c r="F17" t="s">
         <v>30</v>
@@ -1534,16 +1462,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2"/>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="11"/>
       <c r="F18" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.25" customHeight="1">
+    <row r="19" spans="1:6">
       <c r="A19" s="6"/>
       <c r="B19" s="20" t="s">
         <v>85</v>
@@ -1578,7 +1506,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.25" customHeight="1">
+    <row r="22" spans="1:6">
       <c r="A22" s="6"/>
       <c r="B22" s="20" t="s">
         <v>86</v>
@@ -1613,44 +1541,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="6"/>
-      <c r="B25" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="F25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="6"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="F26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="6"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="F27" t="s">
-        <v>98</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B25:B27"/>
+  <mergeCells count="15">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
@@ -1674,10 +1566,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1687,12 +1579,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1702,10 +1594,10 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1718,10 +1610,10 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="4"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
@@ -1731,11 +1623,11 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="4"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
@@ -1745,11 +1637,11 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="17.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
@@ -1759,11 +1651,11 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="17.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -1773,11 +1665,11 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="18">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="9" t="s">
         <v>24</v>
       </c>
@@ -1787,11 +1679,11 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="17.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="9"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
@@ -1899,10 +1791,10 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="2"/>
       <c r="D16" s="10"/>
       <c r="E16" s="1"/>
@@ -1918,10 +1810,10 @@
       <c r="A17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="29"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="11"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
@@ -1932,10 +1824,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3"/>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="11"/>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
@@ -1946,10 +1838,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2"/>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="28"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="11"/>
       <c r="E19" s="1"/>
       <c r="F19" t="s">
@@ -1960,10 +1852,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2"/>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="28"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="11"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
@@ -2042,17 +1934,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.25" customHeight="1">
+    <row r="27" spans="1:8">
       <c r="A27" s="6"/>
       <c r="B27" s="20" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>82</v>
       </c>
       <c r="D27" s="11"/>
       <c r="F27" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2063,7 +1955,7 @@
       </c>
       <c r="D28" s="11"/>
       <c r="F28" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2074,20 +1966,20 @@
       </c>
       <c r="D29" s="11"/>
       <c r="F29" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="6"/>
       <c r="B30" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>82</v>
       </c>
       <c r="D30" s="11"/>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2098,7 +1990,7 @@
       </c>
       <c r="D31" s="11"/>
       <c r="F31" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2109,86 +2001,11 @@
       </c>
       <c r="D32" s="11"/>
       <c r="F32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="6"/>
-      <c r="B33" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="F33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="6"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="F34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="6"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="F35" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="6"/>
-      <c r="B36" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="11"/>
-      <c r="F36" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="6"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" s="11"/>
-      <c r="F37" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="6"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="F38" t="s">
-        <v>104</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B33:B35"/>
+  <mergeCells count="17">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
@@ -2203,19 +2020,21 @@
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2224,12 +2043,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2239,10 +2058,10 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -2255,10 +2074,10 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="4"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
@@ -2268,11 +2087,11 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="4"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
@@ -2282,11 +2101,11 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="17.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
@@ -2296,11 +2115,11 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="17.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -2310,11 +2129,11 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="18">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="9" t="s">
         <v>24</v>
       </c>
@@ -2324,11 +2143,11 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="17.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="9"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
@@ -2408,10 +2227,10 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="27"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="2"/>
       <c r="D14" s="10"/>
       <c r="E14" s="1"/>
@@ -2427,10 +2246,10 @@
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="11"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
@@ -2441,10 +2260,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3"/>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="11"/>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
@@ -2455,10 +2274,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2"/>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="11"/>
       <c r="E17" s="1"/>
       <c r="F17" t="s">
@@ -2469,10 +2288,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2"/>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="11"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
@@ -2551,44 +2370,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="6"/>
-      <c r="B25" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="F25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="6"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="F26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="6"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="F27" t="s">
-        <v>99</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B25:B27"/>
+  <mergeCells count="15">
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -2612,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2625,21 +2408,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -2649,65 +2432,65 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="4"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="12"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="13"/>
       <c r="F5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="13"/>
       <c r="F6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="13"/>
       <c r="F7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="13" t="s">
         <v>24</v>
       </c>
@@ -2779,10 +2562,10 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="2"/>
       <c r="D15" s="15"/>
       <c r="F15" s="1" t="s">
@@ -2796,10 +2579,10 @@
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="31"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="16"/>
       <c r="F16" s="1" t="s">
         <v>25</v>
@@ -2807,10 +2590,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3"/>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="29"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="16"/>
       <c r="F17" t="s">
         <v>51</v>
@@ -2818,10 +2601,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="16"/>
       <c r="F18" t="s">
         <v>48</v>
@@ -2829,10 +2612,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3"/>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="16"/>
       <c r="F19" t="s">
         <v>50</v>
@@ -2846,7 +2629,7 @@
       <c r="C20" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="16"/>
       <c r="F20" t="s">
         <v>71</v>
       </c>
@@ -2857,7 +2640,7 @@
       <c r="C21" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="11"/>
+      <c r="D21" s="16"/>
       <c r="F21" t="s">
         <v>72</v>
       </c>
@@ -2868,7 +2651,7 @@
       <c r="C22" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="16"/>
       <c r="F22" t="s">
         <v>77</v>
       </c>
@@ -2879,7 +2662,7 @@
       <c r="C23" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="16"/>
       <c r="F23" t="s">
         <v>91</v>
       </c>
@@ -2890,7 +2673,7 @@
       <c r="C24" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="11"/>
+      <c r="D24" s="16"/>
       <c r="F24" t="s">
         <v>92</v>
       </c>
@@ -2898,12 +2681,12 @@
     <row r="25" spans="1:6">
       <c r="A25" s="6"/>
       <c r="B25" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="16"/>
       <c r="F25" t="s">
         <v>74</v>
       </c>
@@ -2914,7 +2697,7 @@
       <c r="C26" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="16"/>
       <c r="F26" t="s">
         <v>73</v>
       </c>
@@ -2925,7 +2708,7 @@
       <c r="C27" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="16"/>
       <c r="F27" t="s">
         <v>78</v>
       </c>
@@ -2936,7 +2719,7 @@
       <c r="C28" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="16"/>
       <c r="F28" t="s">
         <v>93</v>
       </c>
@@ -2947,71 +2730,13 @@
       <c r="C29" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="11"/>
+      <c r="D29" s="16"/>
       <c r="F29" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="6"/>
-      <c r="B30" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="F30" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="6"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="F31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="6"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="F32" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="18"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="F33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="18"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="F34" t="s">
-        <v>107</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B30:B34"/>
+  <mergeCells count="15">
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -3029,24 +2754,16 @@
     <mergeCell ref="B20:B24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D17">
-      <formula1>"地上,地下"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19 D17">
-      <formula1>"h≤24,24＜h≤50,50＜h≤100"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3056,21 +2773,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -3080,65 +2797,65 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="4"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="12"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="13"/>
       <c r="F5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="13"/>
       <c r="F6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="13"/>
       <c r="F7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="13" t="s">
         <v>24</v>
       </c>
@@ -3210,10 +2927,10 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="2"/>
       <c r="D15" s="15"/>
       <c r="F15" s="1" t="s">
@@ -3227,44 +2944,44 @@
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="11"/>
       <c r="F16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3"/>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="11"/>
       <c r="F17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="16"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="11"/>
       <c r="F18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3"/>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="16"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="11"/>
       <c r="F19" t="s">
         <v>50</v>
       </c>
@@ -3329,7 +3046,7 @@
     <row r="25" spans="1:6">
       <c r="A25" s="6"/>
       <c r="B25" s="20" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>82</v>
@@ -3383,66 +3100,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="6"/>
-      <c r="B30" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="F30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="6"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="F31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="6"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="F32" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="18"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="F33" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="18"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="F34" t="s">
-        <v>110</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B30:B34"/>
+  <mergeCells count="15">
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -3460,14 +3119,6 @@
     <mergeCell ref="B20:B24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19 D17">
-      <formula1>"h≤24,24＜h≤50,50＜h≤100"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D17">
-      <formula1>"地上,地下"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3477,7 +3128,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3486,21 +3137,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -3510,21 +3161,21 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="4"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="12"/>
       <c r="F4" s="1" t="s">
         <v>63</v>
@@ -3534,22 +3185,22 @@
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="11"/>
       <c r="F5" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3"/>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="11"/>
       <c r="F6" t="s">
         <v>62</v>
       </c>
@@ -3564,24 +3215,16 @@
     <mergeCell ref="A4:C4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6">
-      <formula1>"地上,地下"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6">
-      <formula1>"h≤24,24＜h≤50,50＜h≤100"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D7:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3590,21 +3233,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -3614,21 +3257,21 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="4"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="12"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
@@ -3728,44 +3371,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="18"/>
-      <c r="B13" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="F13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="18"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="F14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="18"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="F15" t="s">
-        <v>99</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B13:B15"/>
+  <mergeCells count="6">
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>

</xml_diff>

<commit_message>
Update SmokeProofScenario 修正错误 门的数量默认3个
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/DesignData/SmokeProofScenario.xlsx
+++ b/AutoLoader/Contents/Support/DesignData/SmokeProofScenario.xlsx
@@ -46,7 +46,7 @@
     <definedName name="valveAf">消防电梯前室!#REF!</definedName>
     <definedName name="Width_Valve">消防电梯前室!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="125">
   <si>
     <t>系统名称</t>
   </si>
@@ -638,27 +638,155 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>高度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宽度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前室疏散门1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前室疏散门2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楼梯间疏散门1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楼梯间疏散门2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>门缝宽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>形式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crack_Door_Q1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type_Door_Q1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crack_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前室疏散门3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楼梯间疏散门3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height_Door_L3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width_Door_L3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_Door_L3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_Door_L1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height_Door_L2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Width_Door_L2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Height_Door_L2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宽度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前室疏散门1</t>
+    <t>Height_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crack_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type_Door_Q3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -666,35 +794,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>楼梯间疏散门1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>楼梯间疏散门2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>门缝宽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>形式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crack_Door_Q1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type_Door_Q1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crack_Door_Q2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type_Door_Q2</t>
+    <t>前室疏散门3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height_Door_Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crack_Door_Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type_Door_Q3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -702,10 +822,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
-    <numFmt numFmtId="178" formatCode="0.000"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -895,49 +1013,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -948,12 +1065,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -968,10 +1079,16 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1254,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -1269,22 +1386,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="10"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
@@ -1293,131 +1410,131 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="10"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="9"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="17"/>
       <c r="F5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="9"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="17"/>
       <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="17"/>
       <c r="F8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="18"/>
       <c r="F9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="18"/>
       <c r="F10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="18"/>
       <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="19"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="19"/>
       <c r="F13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="20"/>
       <c r="F14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1426,123 +1543,159 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="11"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="13"/>
       <c r="F15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3"/>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="13"/>
       <c r="F16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2"/>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="13"/>
       <c r="F17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2"/>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="13"/>
       <c r="F18" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="6"/>
-      <c r="B19" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="11"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="13"/>
       <c r="F19" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="6"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="11"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="13"/>
       <c r="F20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="11"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="13"/>
       <c r="F21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="6"/>
-      <c r="B22" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="F22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="5"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="F23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="5"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="F22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="6"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="F23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="6"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="11"/>
+      <c r="D24" s="13"/>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="5"/>
+      <c r="B25" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="F25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="5"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="5"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="F27" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B25:B27"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
@@ -1566,10 +1719,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1579,12 +1732,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1594,11 +1747,11 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -1610,11 +1763,11 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
@@ -1623,12 +1776,12 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
@@ -1637,12 +1790,12 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="17.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="9"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>38</v>
@@ -1651,12 +1804,12 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="17.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="9"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>39</v>
@@ -1665,12 +1818,12 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="18">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="1"/>
@@ -1679,12 +1832,12 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="17.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
         <v>40</v>
@@ -1694,11 +1847,11 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
         <v>27</v>
@@ -1708,11 +1861,11 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>33</v>
@@ -1722,11 +1875,11 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
         <v>32</v>
@@ -1736,11 +1889,11 @@
     </row>
     <row r="12" spans="1:8" ht="17.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
@@ -1750,11 +1903,11 @@
     </row>
     <row r="13" spans="1:8" ht="17.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
         <v>35</v>
@@ -1764,11 +1917,11 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
         <v>43</v>
@@ -1778,11 +1931,11 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
         <v>59</v>
@@ -1791,12 +1944,12 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
         <v>36</v>
@@ -1807,14 +1960,14 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
         <v>25</v>
@@ -1824,11 +1977,11 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3"/>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
         <v>26</v>
@@ -1838,11 +1991,11 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2"/>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="11"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="1"/>
       <c r="F19" t="s">
         <v>30</v>
@@ -1852,11 +2005,11 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2"/>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="11"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
         <v>31</v>
@@ -1865,147 +2018,221 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="6"/>
-      <c r="B21" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="11"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="13"/>
       <c r="F21" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="6"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="11"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="13"/>
       <c r="F22" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="6"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="11"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="13"/>
       <c r="F23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="6"/>
-      <c r="B24" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="F25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="F24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="6"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="F25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="6"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="13"/>
       <c r="F26" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="6"/>
-      <c r="B27" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="17" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="F27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="5"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="F28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="5"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="F27" t="s">
+      <c r="D29" s="13"/>
+      <c r="F29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="5"/>
+      <c r="B30" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="F30" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="6"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="F28" t="s">
+    <row r="31" spans="1:8">
+      <c r="A31" s="5"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="F31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="6"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="F29" t="s">
+    <row r="32" spans="1:8">
+      <c r="A32" s="5"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="F32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="5"/>
+      <c r="B33" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="F33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="5"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="F34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="5"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="F35" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="6"/>
-      <c r="B30" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="17" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="5"/>
+      <c r="B36" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="F36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="5"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="F37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="5"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="F30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="6"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="F31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="6"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="F32" t="s">
-        <v>79</v>
+      <c r="D38" s="13"/>
+      <c r="F38" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B36:B38"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
@@ -2017,12 +2244,10 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
     <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2031,10 +2256,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2043,12 +2268,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2058,11 +2283,11 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -2074,11 +2299,11 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
@@ -2087,12 +2312,12 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
@@ -2101,12 +2326,12 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="17.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="9"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>38</v>
@@ -2115,12 +2340,12 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="17.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="9"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>39</v>
@@ -2129,12 +2354,12 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="18">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="1"/>
@@ -2143,12 +2368,12 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="17.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
         <v>40</v>
@@ -2158,11 +2383,11 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
         <v>27</v>
@@ -2172,11 +2397,11 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>33</v>
@@ -2186,11 +2411,11 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
         <v>32</v>
@@ -2200,11 +2425,11 @@
     </row>
     <row r="12" spans="1:8" ht="17.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
@@ -2214,11 +2439,11 @@
     </row>
     <row r="13" spans="1:8" ht="17.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
         <v>35</v>
@@ -2227,12 +2452,12 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
         <v>36</v>
@@ -2243,14 +2468,14 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="11"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
         <v>25</v>
@@ -2260,11 +2485,11 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3"/>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
         <v>26</v>
@@ -2274,11 +2499,11 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2"/>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="1"/>
       <c r="F17" t="s">
         <v>30</v>
@@ -2288,11 +2513,11 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2"/>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
         <v>31</v>
@@ -2301,77 +2526,113 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="6"/>
-      <c r="B19" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="11"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="13"/>
       <c r="F19" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="6"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="11"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="13"/>
       <c r="F20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="6"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="11"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="13"/>
       <c r="F21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="6"/>
-      <c r="B22" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="F22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="5"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="F23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="5"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="F22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="6"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="F23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="6"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="11"/>
+      <c r="D24" s="13"/>
       <c r="F24" t="s">
         <v>78</v>
       </c>
     </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5"/>
+      <c r="B25" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="F25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="5"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="F27" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B25:B27"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -2395,10 +2656,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2419,11 +2680,11 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="10"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2432,66 +2693,66 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="11"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="13"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="14"/>
       <c r="F5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="14"/>
       <c r="F6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="14"/>
       <c r="F7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="13" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2501,7 +2762,7 @@
       <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="12"/>
       <c r="F9" t="s">
         <v>27</v>
       </c>
@@ -2512,7 +2773,7 @@
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="12"/>
       <c r="F10" t="s">
         <v>33</v>
       </c>
@@ -2523,7 +2784,7 @@
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="12"/>
       <c r="F11" t="s">
         <v>32</v>
       </c>
@@ -2534,7 +2795,7 @@
       <c r="C12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="12"/>
       <c r="F12" t="s">
         <v>53</v>
       </c>
@@ -2545,7 +2806,7 @@
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="12"/>
       <c r="F13" t="s">
         <v>56</v>
       </c>
@@ -2556,16 +2817,16 @@
       <c r="C14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="12"/>
       <c r="F14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="2"/>
       <c r="D15" s="15"/>
       <c r="F15" s="1" t="s">
@@ -2576,13 +2837,13 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="30"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="16"/>
       <c r="F16" s="1" t="s">
         <v>25</v>
@@ -2590,10 +2851,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3"/>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="16"/>
       <c r="F17" t="s">
         <v>51</v>
@@ -2601,10 +2862,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="16"/>
       <c r="F18" t="s">
         <v>48</v>
@@ -2612,22 +2873,22 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3"/>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="23"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="16"/>
       <c r="F19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>82</v>
+      <c r="A20" s="5"/>
+      <c r="B20" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="D20" s="16"/>
       <c r="F20" t="s">
@@ -2635,10 +2896,10 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="17" t="s">
-        <v>83</v>
+      <c r="A21" s="5"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="D21" s="16"/>
       <c r="F21" t="s">
@@ -2646,10 +2907,10 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="6"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="17" t="s">
-        <v>84</v>
+      <c r="A22" s="5"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D22" s="16"/>
       <c r="F22" t="s">
@@ -2657,34 +2918,34 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="18"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="19" t="s">
-        <v>89</v>
+      <c r="A23" s="8"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="D23" s="16"/>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="18"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="19" t="s">
-        <v>90</v>
+      <c r="A24" s="8"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="D24" s="16"/>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="6"/>
-      <c r="B25" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>82</v>
+      <c r="A25" s="5"/>
+      <c r="B25" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="D25" s="16"/>
       <c r="F25" t="s">
@@ -2692,10 +2953,10 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="6"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="17" t="s">
-        <v>83</v>
+      <c r="A26" s="5"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="D26" s="16"/>
       <c r="F26" t="s">
@@ -2703,10 +2964,10 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="6"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="17" t="s">
-        <v>84</v>
+      <c r="A27" s="5"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D27" s="16"/>
       <c r="F27" t="s">
@@ -2714,29 +2975,87 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="18"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="19" t="s">
-        <v>89</v>
+      <c r="A28" s="8"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="D28" s="16"/>
       <c r="F28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="18"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="19" t="s">
-        <v>90</v>
+      <c r="A29" s="8"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="D29" s="16"/>
       <c r="F29" t="s">
-        <v>94</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="5"/>
+      <c r="B30" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="F30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="F31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="5"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="16"/>
+      <c r="F32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="8"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="F33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="8"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="16"/>
+      <c r="F34" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B30:B34"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -2760,10 +3079,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2784,11 +3103,11 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="10"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2797,66 +3116,66 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="11"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="13"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="14"/>
       <c r="F5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="14"/>
       <c r="F6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="14"/>
       <c r="F7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="13" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2866,7 +3185,7 @@
       <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="12"/>
       <c r="F9" t="s">
         <v>27</v>
       </c>
@@ -2877,7 +3196,7 @@
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="12"/>
       <c r="F10" t="s">
         <v>33</v>
       </c>
@@ -2888,7 +3207,7 @@
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="12"/>
       <c r="F11" t="s">
         <v>32</v>
       </c>
@@ -2899,7 +3218,7 @@
       <c r="C12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="12"/>
       <c r="F12" t="s">
         <v>53</v>
       </c>
@@ -2910,7 +3229,7 @@
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="12"/>
       <c r="F13" t="s">
         <v>56</v>
       </c>
@@ -2921,16 +3240,16 @@
       <c r="C14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="12"/>
       <c r="F14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="2"/>
       <c r="D15" s="15"/>
       <c r="F15" s="1" t="s">
@@ -2941,167 +3260,225 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="13"/>
       <c r="F16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3"/>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="13"/>
       <c r="F17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="13"/>
       <c r="F18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3"/>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="11"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="13"/>
       <c r="F19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="6"/>
-      <c r="B20" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="11"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="13"/>
       <c r="F20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="11"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="13"/>
       <c r="F21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="6"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="11"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="13"/>
       <c r="F22" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="18"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="19" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="F23" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="F23" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="18"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="19" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="F24" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="F24" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="6"/>
-      <c r="B25" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="11"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="13"/>
       <c r="F25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="6"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="11"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="13"/>
       <c r="F26" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="6"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="11"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="13"/>
       <c r="F27" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="18"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="11"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="13"/>
       <c r="F28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="8"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="F29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="5"/>
+      <c r="B30" s="21" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="18"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="F29" t="s">
-        <v>94</v>
+      <c r="C30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="F30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="F31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="5"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="F32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="8"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="F33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="8"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="F34" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B30:B34"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -3128,7 +3505,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3148,11 +3525,11 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="10"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
@@ -3161,46 +3538,46 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="11"/>
       <c r="F4" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="11"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="13"/>
       <c r="F5" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3"/>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="13"/>
       <c r="F6" t="s">
         <v>62</v>
       </c>
@@ -3221,10 +3598,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D7:D12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3244,11 +3621,11 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="10"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
@@ -3257,22 +3634,22 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="11"/>
       <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
@@ -3283,7 +3660,7 @@
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="12"/>
       <c r="F5" t="s">
         <v>27</v>
       </c>
@@ -3294,85 +3671,112 @@
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="12"/>
       <c r="F6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="11"/>
+      <c r="B7" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="13"/>
       <c r="F7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="18"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="11"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="13"/>
       <c r="F8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="18"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="11"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="13"/>
       <c r="F9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="18"/>
-      <c r="B10" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="8"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="8"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="F10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="18"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="F11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="18"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="13"/>
       <c r="F12" t="s">
         <v>78</v>
       </c>
     </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="8"/>
+      <c r="B13" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="8"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="8"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
@@ -3382,5 +3786,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>